<commit_message>
Fix Frontend_Table_Description.xlsx generation COLUMN_TYPE
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description_generated.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description_generated.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="403">
   <si>
     <t xml:space="preserve">TABLE_NAME</t>
   </si>
@@ -89,12 +89,18 @@
     <t xml:space="preserve">Geburtsdatum</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
     <t xml:space="preserve">pat_aktuell_alter</t>
   </si>
   <si>
     <t xml:space="preserve">aktuelles Patientenalter (Jahre)</t>
   </si>
   <si>
+    <t xml:space="preserve">double precision</t>
+  </si>
+  <si>
     <t xml:space="preserve">pat_geschlecht</t>
   </si>
   <si>
@@ -144,6 +150,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aufnahmedatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
   </si>
   <si>
     <t xml:space="preserve">fall_zimmernr</t>
@@ -315,6 +324,9 @@
     <t xml:space="preserve">genaue Dauer in Minuten</t>
   </si>
   <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
     <t xml:space="preserve">meda_notiz</t>
   </si>
   <si>
@@ -1071,9 +1083,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aggregation der Felder 27-33: Anzahl der Felder mit Ausprägung &gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double precision</t>
   </si>
   <si>
     <t xml:space="preserve">risikofaktor_complete</t>
@@ -1684,7 +1693,7 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -1692,13 +1701,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -1706,10 +1715,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1720,10 +1729,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1731,7 +1740,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1790,10 +1799,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1804,10 +1813,10 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1818,10 +1827,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -1832,10 +1841,10 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -1846,10 +1855,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1860,13 +1869,13 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24">
@@ -1874,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1888,10 +1897,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1902,13 +1911,13 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27">
@@ -1916,10 +1925,10 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1930,13 +1939,13 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29">
@@ -1944,10 +1953,10 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1958,13 +1967,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31">
@@ -1972,10 +1981,10 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1986,13 +1995,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
@@ -2000,10 +2009,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -2011,7 +2020,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -2070,10 +2079,10 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -2084,10 +2093,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -2098,10 +2107,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -2112,10 +2121,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -2126,10 +2135,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -2140,13 +2149,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44">
@@ -2154,13 +2163,13 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45">
@@ -2168,10 +2177,10 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -2182,13 +2191,13 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47">
@@ -2196,10 +2205,10 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -2210,13 +2219,13 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49">
@@ -2224,10 +2233,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
@@ -2238,10 +2247,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -2252,10 +2261,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -2266,10 +2275,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -2280,10 +2289,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -2294,10 +2303,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -2308,10 +2317,10 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -2322,10 +2331,10 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -2336,10 +2345,10 @@
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -2350,13 +2359,13 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59">
@@ -2364,10 +2373,10 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -2378,10 +2387,10 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -2389,7 +2398,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
@@ -2448,10 +2457,10 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -2462,10 +2471,10 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -2476,10 +2485,10 @@
         <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -2490,10 +2499,10 @@
         <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -2504,13 +2513,13 @@
         <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70">
@@ -2518,10 +2527,10 @@
         <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -2532,10 +2541,10 @@
         <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -2546,10 +2555,10 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C72" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -2560,10 +2569,10 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -2574,10 +2583,10 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C74" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -2588,10 +2597,10 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -2602,10 +2611,10 @@
         <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C76" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -2616,10 +2625,10 @@
         <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C77" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -2630,10 +2639,10 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -2644,10 +2653,10 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -2658,10 +2667,10 @@
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -2672,10 +2681,10 @@
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -2686,10 +2695,10 @@
         <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C82" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -2700,10 +2709,10 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -2714,10 +2723,10 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C84" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -2728,10 +2737,10 @@
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -2742,10 +2751,10 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C86" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
@@ -2756,10 +2765,10 @@
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C87" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
@@ -2770,10 +2779,10 @@
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C88" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
@@ -2784,10 +2793,10 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C89" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
@@ -2798,10 +2807,10 @@
         <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C90" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
@@ -2812,10 +2821,10 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C91" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
@@ -2826,10 +2835,10 @@
         <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C92" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
@@ -2840,10 +2849,10 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C93" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
@@ -2854,10 +2863,10 @@
         <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D94" t="s">
         <v>7</v>
@@ -2868,10 +2877,10 @@
         <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C95" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D95" t="s">
         <v>7</v>
@@ -2882,10 +2891,10 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C96" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D96" t="s">
         <v>7</v>
@@ -2896,10 +2905,10 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C97" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
@@ -2910,10 +2919,10 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C98" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
@@ -2924,10 +2933,10 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C99" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D99" t="s">
         <v>7</v>
@@ -2938,10 +2947,10 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C100" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -2952,10 +2961,10 @@
         <v>8</v>
       </c>
       <c r="B101" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C101" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D101" t="s">
         <v>7</v>
@@ -2966,10 +2975,10 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C102" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D102" t="s">
         <v>7</v>
@@ -2980,10 +2989,10 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C103" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D103" t="s">
         <v>7</v>
@@ -2994,10 +3003,10 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C104" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D104" t="s">
         <v>7</v>
@@ -3008,10 +3017,10 @@
         <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C105" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D105" t="s">
         <v>7</v>
@@ -3022,10 +3031,10 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D106" t="s">
         <v>7</v>
@@ -3036,10 +3045,10 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C107" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
@@ -3050,10 +3059,10 @@
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C108" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
@@ -3064,10 +3073,10 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C109" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D109" t="s">
         <v>7</v>
@@ -3078,10 +3087,10 @@
         <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C110" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D110" t="s">
         <v>7</v>
@@ -3092,10 +3101,10 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C111" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
@@ -3106,10 +3115,10 @@
         <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C112" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D112" t="s">
         <v>7</v>
@@ -3120,10 +3129,10 @@
         <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C113" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D113" t="s">
         <v>7</v>
@@ -3134,10 +3143,10 @@
         <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
@@ -3148,10 +3157,10 @@
         <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C115" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D115" t="s">
         <v>7</v>
@@ -3162,10 +3171,10 @@
         <v>8</v>
       </c>
       <c r="B116" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C116" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D116" t="s">
         <v>7</v>
@@ -3176,10 +3185,10 @@
         <v>8</v>
       </c>
       <c r="B117" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C117" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D117" t="s">
         <v>7</v>
@@ -3190,10 +3199,10 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C118" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D118" t="s">
         <v>7</v>
@@ -3204,10 +3213,10 @@
         <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C119" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
@@ -3218,10 +3227,10 @@
         <v>8</v>
       </c>
       <c r="B120" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C120" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -3232,10 +3241,10 @@
         <v>8</v>
       </c>
       <c r="B121" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C121" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
@@ -3246,10 +3255,10 @@
         <v>8</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C122" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
@@ -3260,10 +3269,10 @@
         <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C123" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D123" t="s">
         <v>7</v>
@@ -3274,10 +3283,10 @@
         <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C124" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D124" t="s">
         <v>7</v>
@@ -3288,10 +3297,10 @@
         <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C125" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D125" t="s">
         <v>7</v>
@@ -3302,10 +3311,10 @@
         <v>8</v>
       </c>
       <c r="B126" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C126" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D126" t="s">
         <v>7</v>
@@ -3316,10 +3325,10 @@
         <v>8</v>
       </c>
       <c r="B127" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C127" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D127" t="s">
         <v>7</v>
@@ -3330,10 +3339,10 @@
         <v>8</v>
       </c>
       <c r="B128" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C128" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
@@ -3344,10 +3353,10 @@
         <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C129" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D129" t="s">
         <v>7</v>
@@ -3358,10 +3367,10 @@
         <v>8</v>
       </c>
       <c r="B130" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C130" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D130" t="s">
         <v>7</v>
@@ -3372,10 +3381,10 @@
         <v>8</v>
       </c>
       <c r="B131" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C131" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D131" t="s">
         <v>7</v>
@@ -3386,10 +3395,10 @@
         <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C132" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
@@ -3400,10 +3409,10 @@
         <v>8</v>
       </c>
       <c r="B133" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C133" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D133" t="s">
         <v>7</v>
@@ -3414,10 +3423,10 @@
         <v>8</v>
       </c>
       <c r="B134" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D134" t="s">
         <v>7</v>
@@ -3428,10 +3437,10 @@
         <v>8</v>
       </c>
       <c r="B135" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C135" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D135" t="s">
         <v>7</v>
@@ -3442,10 +3451,10 @@
         <v>8</v>
       </c>
       <c r="B136" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C136" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D136" t="s">
         <v>7</v>
@@ -3453,7 +3462,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
@@ -3512,10 +3521,10 @@
         <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C141" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D141" t="s">
         <v>7</v>
@@ -3526,10 +3535,10 @@
         <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C142" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D142" t="s">
         <v>7</v>
@@ -3540,10 +3549,10 @@
         <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C143" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D143" t="s">
         <v>7</v>
@@ -3554,13 +3563,13 @@
         <v>8</v>
       </c>
       <c r="B144" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C144" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D144" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145">
@@ -3568,10 +3577,10 @@
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C145" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D145" t="s">
         <v>7</v>
@@ -3582,10 +3591,10 @@
         <v>8</v>
       </c>
       <c r="B146" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C146" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
@@ -3596,10 +3605,10 @@
         <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C147" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D147" t="s">
         <v>7</v>
@@ -3610,10 +3619,10 @@
         <v>8</v>
       </c>
       <c r="B148" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C148" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D148" t="s">
         <v>7</v>
@@ -3624,10 +3633,10 @@
         <v>8</v>
       </c>
       <c r="B149" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C149" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D149" t="s">
         <v>7</v>
@@ -3638,10 +3647,10 @@
         <v>8</v>
       </c>
       <c r="B150" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C150" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D150" t="s">
         <v>7</v>
@@ -3652,10 +3661,10 @@
         <v>8</v>
       </c>
       <c r="B151" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C151" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D151" t="s">
         <v>7</v>
@@ -3666,10 +3675,10 @@
         <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C152" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D152" t="s">
         <v>7</v>
@@ -3680,10 +3689,10 @@
         <v>8</v>
       </c>
       <c r="B153" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C153" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D153" t="s">
         <v>7</v>
@@ -3694,10 +3703,10 @@
         <v>8</v>
       </c>
       <c r="B154" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C154" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D154" t="s">
         <v>7</v>
@@ -3708,10 +3717,10 @@
         <v>8</v>
       </c>
       <c r="B155" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C155" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D155" t="s">
         <v>7</v>
@@ -3722,10 +3731,10 @@
         <v>8</v>
       </c>
       <c r="B156" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C156" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D156" t="s">
         <v>7</v>
@@ -3736,10 +3745,10 @@
         <v>8</v>
       </c>
       <c r="B157" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C157" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D157" t="s">
         <v>7</v>
@@ -3750,10 +3759,10 @@
         <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C158" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D158" t="s">
         <v>7</v>
@@ -3764,10 +3773,10 @@
         <v>8</v>
       </c>
       <c r="B159" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C159" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D159" t="s">
         <v>7</v>
@@ -3778,10 +3787,10 @@
         <v>8</v>
       </c>
       <c r="B160" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C160" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D160" t="s">
         <v>7</v>
@@ -3792,10 +3801,10 @@
         <v>8</v>
       </c>
       <c r="B161" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C161" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D161" t="s">
         <v>7</v>
@@ -3806,10 +3815,10 @@
         <v>8</v>
       </c>
       <c r="B162" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C162" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D162" t="s">
         <v>7</v>
@@ -3820,10 +3829,10 @@
         <v>8</v>
       </c>
       <c r="B163" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C163" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D163" t="s">
         <v>7</v>
@@ -3834,10 +3843,10 @@
         <v>8</v>
       </c>
       <c r="B164" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C164" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D164" t="s">
         <v>7</v>
@@ -3848,10 +3857,10 @@
         <v>8</v>
       </c>
       <c r="B165" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C165" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D165" t="s">
         <v>7</v>
@@ -3862,10 +3871,10 @@
         <v>8</v>
       </c>
       <c r="B166" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C166" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D166" t="s">
         <v>7</v>
@@ -3876,10 +3885,10 @@
         <v>8</v>
       </c>
       <c r="B167" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C167" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D167" t="s">
         <v>7</v>
@@ -3890,10 +3899,10 @@
         <v>8</v>
       </c>
       <c r="B168" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C168" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D168" t="s">
         <v>7</v>
@@ -3904,10 +3913,10 @@
         <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C169" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D169" t="s">
         <v>7</v>
@@ -3918,10 +3927,10 @@
         <v>8</v>
       </c>
       <c r="B170" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C170" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D170" t="s">
         <v>7</v>
@@ -3932,10 +3941,10 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C171" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D171" t="s">
         <v>7</v>
@@ -3946,10 +3955,10 @@
         <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C172" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D172" t="s">
         <v>7</v>
@@ -3960,10 +3969,10 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C173" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D173" t="s">
         <v>7</v>
@@ -3974,10 +3983,10 @@
         <v>8</v>
       </c>
       <c r="B174" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C174" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D174" t="s">
         <v>7</v>
@@ -3988,13 +3997,13 @@
         <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C175" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D175" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="176">
@@ -4002,10 +4011,10 @@
         <v>8</v>
       </c>
       <c r="B176" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C176" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D176" t="s">
         <v>7</v>
@@ -4016,10 +4025,10 @@
         <v>8</v>
       </c>
       <c r="B177" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C177" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D177" t="s">
         <v>7</v>
@@ -4030,10 +4039,10 @@
         <v>8</v>
       </c>
       <c r="B178" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C178" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D178" t="s">
         <v>7</v>
@@ -4044,10 +4053,10 @@
         <v>8</v>
       </c>
       <c r="B179" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C179" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D179" t="s">
         <v>7</v>
@@ -4058,10 +4067,10 @@
         <v>8</v>
       </c>
       <c r="B180" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C180" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D180" t="s">
         <v>7</v>
@@ -4072,10 +4081,10 @@
         <v>8</v>
       </c>
       <c r="B181" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C181" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D181" t="s">
         <v>7</v>
@@ -4086,10 +4095,10 @@
         <v>8</v>
       </c>
       <c r="B182" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C182" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D182" t="s">
         <v>7</v>
@@ -4100,10 +4109,10 @@
         <v>8</v>
       </c>
       <c r="B183" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C183" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D183" t="s">
         <v>7</v>
@@ -4114,10 +4123,10 @@
         <v>8</v>
       </c>
       <c r="B184" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C184" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D184" t="s">
         <v>7</v>
@@ -4128,10 +4137,10 @@
         <v>8</v>
       </c>
       <c r="B185" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C185" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D185" t="s">
         <v>7</v>
@@ -4142,10 +4151,10 @@
         <v>8</v>
       </c>
       <c r="B186" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C186" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D186" t="s">
         <v>7</v>
@@ -4156,10 +4165,10 @@
         <v>8</v>
       </c>
       <c r="B187" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C187" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D187" t="s">
         <v>7</v>
@@ -4170,10 +4179,10 @@
         <v>8</v>
       </c>
       <c r="B188" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C188" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D188" t="s">
         <v>7</v>
@@ -4184,10 +4193,10 @@
         <v>8</v>
       </c>
       <c r="B189" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C189" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D189" t="s">
         <v>7</v>
@@ -4198,10 +4207,10 @@
         <v>8</v>
       </c>
       <c r="B190" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C190" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D190" t="s">
         <v>7</v>
@@ -4212,10 +4221,10 @@
         <v>8</v>
       </c>
       <c r="B191" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C191" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D191" t="s">
         <v>7</v>
@@ -4226,10 +4235,10 @@
         <v>8</v>
       </c>
       <c r="B192" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C192" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D192" t="s">
         <v>7</v>
@@ -4240,10 +4249,10 @@
         <v>8</v>
       </c>
       <c r="B193" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C193" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D193" t="s">
         <v>7</v>
@@ -4254,10 +4263,10 @@
         <v>8</v>
       </c>
       <c r="B194" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C194" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D194" t="s">
         <v>7</v>
@@ -4268,10 +4277,10 @@
         <v>8</v>
       </c>
       <c r="B195" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C195" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D195" t="s">
         <v>7</v>
@@ -4282,10 +4291,10 @@
         <v>8</v>
       </c>
       <c r="B196" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C196" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D196" t="s">
         <v>7</v>
@@ -4296,10 +4305,10 @@
         <v>8</v>
       </c>
       <c r="B197" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C197" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D197" t="s">
         <v>7</v>
@@ -4310,10 +4319,10 @@
         <v>8</v>
       </c>
       <c r="B198" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C198" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D198" t="s">
         <v>7</v>
@@ -4324,10 +4333,10 @@
         <v>8</v>
       </c>
       <c r="B199" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C199" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D199" t="s">
         <v>7</v>
@@ -4338,10 +4347,10 @@
         <v>8</v>
       </c>
       <c r="B200" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C200" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D200" t="s">
         <v>7</v>
@@ -4352,10 +4361,10 @@
         <v>8</v>
       </c>
       <c r="B201" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="C201" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D201" t="s">
         <v>7</v>
@@ -4366,10 +4375,10 @@
         <v>8</v>
       </c>
       <c r="B202" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C202" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D202" t="s">
         <v>7</v>
@@ -4380,10 +4389,10 @@
         <v>8</v>
       </c>
       <c r="B203" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C203" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D203" t="s">
         <v>7</v>
@@ -4394,10 +4403,10 @@
         <v>8</v>
       </c>
       <c r="B204" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C204" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D204" t="s">
         <v>7</v>
@@ -4405,7 +4414,7 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B205" t="s">
         <v>5</v>
@@ -4464,13 +4473,13 @@
         <v>8</v>
       </c>
       <c r="B209" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C209" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D209" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="210">
@@ -4478,13 +4487,13 @@
         <v>8</v>
       </c>
       <c r="B210" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C210" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D210" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="211">
@@ -4492,13 +4501,13 @@
         <v>8</v>
       </c>
       <c r="B211" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C211" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D211" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="212">
@@ -4506,13 +4515,13 @@
         <v>8</v>
       </c>
       <c r="B212" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C212" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="D212" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="213">
@@ -4520,13 +4529,13 @@
         <v>8</v>
       </c>
       <c r="B213" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C213" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D213" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="214">
@@ -4534,13 +4543,13 @@
         <v>8</v>
       </c>
       <c r="B214" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C214" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D214" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="215">
@@ -4548,13 +4557,13 @@
         <v>8</v>
       </c>
       <c r="B215" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C215" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D215" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="216">
@@ -4562,13 +4571,13 @@
         <v>8</v>
       </c>
       <c r="B216" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C216" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D216" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="217">
@@ -4576,13 +4585,13 @@
         <v>8</v>
       </c>
       <c r="B217" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C217" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D217" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="218">
@@ -4590,13 +4599,13 @@
         <v>8</v>
       </c>
       <c r="B218" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C218" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D218" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="219">
@@ -4604,13 +4613,13 @@
         <v>8</v>
       </c>
       <c r="B219" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C219" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D219" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="220">
@@ -4618,13 +4627,13 @@
         <v>8</v>
       </c>
       <c r="B220" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C220" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D220" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="221">
@@ -4632,13 +4641,13 @@
         <v>8</v>
       </c>
       <c r="B221" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C221" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D221" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="222">
@@ -4646,13 +4655,13 @@
         <v>8</v>
       </c>
       <c r="B222" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C222" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D222" t="s">
-        <v>352</v>
+        <v>28</v>
       </c>
     </row>
     <row r="223">
@@ -4660,10 +4669,10 @@
         <v>8</v>
       </c>
       <c r="B223" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C223" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D223" t="s">
         <v>7</v>
@@ -4671,7 +4680,7 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B224" t="s">
         <v>5</v>
@@ -4730,13 +4739,13 @@
         <v>8</v>
       </c>
       <c r="B228" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C228" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D228" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="229">
@@ -4744,13 +4753,13 @@
         <v>8</v>
       </c>
       <c r="B229" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C229" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D229" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="230">
@@ -4758,13 +4767,13 @@
         <v>8</v>
       </c>
       <c r="B230" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C230" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D230" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="231">
@@ -4772,13 +4781,13 @@
         <v>8</v>
       </c>
       <c r="B231" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C231" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D231" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="232">
@@ -4786,13 +4795,13 @@
         <v>8</v>
       </c>
       <c r="B232" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C232" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D232" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="233">
@@ -4800,13 +4809,13 @@
         <v>8</v>
       </c>
       <c r="B233" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C233" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D233" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="234">
@@ -4814,13 +4823,13 @@
         <v>8</v>
       </c>
       <c r="B234" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C234" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D234" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="235">
@@ -4828,13 +4837,13 @@
         <v>8</v>
       </c>
       <c r="B235" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C235" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D235" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="236">
@@ -4842,13 +4851,13 @@
         <v>8</v>
       </c>
       <c r="B236" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C236" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="D236" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="237">
@@ -4856,13 +4865,13 @@
         <v>8</v>
       </c>
       <c r="B237" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C237" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D237" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="238">
@@ -4870,13 +4879,13 @@
         <v>8</v>
       </c>
       <c r="B238" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C238" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="D238" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="239">
@@ -4884,13 +4893,13 @@
         <v>8</v>
       </c>
       <c r="B239" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C239" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D239" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="240">
@@ -4898,13 +4907,13 @@
         <v>8</v>
       </c>
       <c r="B240" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C240" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D240" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="241">
@@ -4912,13 +4921,13 @@
         <v>8</v>
       </c>
       <c r="B241" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C241" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D241" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="242">
@@ -4926,13 +4935,13 @@
         <v>8</v>
       </c>
       <c r="B242" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C242" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D242" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="243">
@@ -4940,13 +4949,13 @@
         <v>8</v>
       </c>
       <c r="B243" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C243" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D243" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="244">
@@ -4954,13 +4963,13 @@
         <v>8</v>
       </c>
       <c r="B244" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C244" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D244" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="245">
@@ -4968,13 +4977,13 @@
         <v>8</v>
       </c>
       <c r="B245" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C245" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D245" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="246">
@@ -4982,13 +4991,13 @@
         <v>8</v>
       </c>
       <c r="B246" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C246" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D246" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="247">
@@ -4996,13 +5005,13 @@
         <v>8</v>
       </c>
       <c r="B247" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C247" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D247" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="248">
@@ -5010,13 +5019,13 @@
         <v>8</v>
       </c>
       <c r="B248" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C248" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="D248" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="249">
@@ -5024,13 +5033,13 @@
         <v>8</v>
       </c>
       <c r="B249" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C249" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="D249" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="250">
@@ -5038,10 +5047,10 @@
         <v>8</v>
       </c>
       <c r="B250" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C250" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D250" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Update Frontend Data Dictionary + generated Table Description
</commit_message>
<xml_diff>
--- a/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description_generated.xlsx
+++ b/R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description_generated.xlsx
@@ -122,6 +122,9 @@
     <t xml:space="preserve">verstecktes Feld für patient_id_fk</t>
   </si>
   <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
     <t xml:space="preserve">fall_pat_id</t>
   </si>
   <si>
@@ -322,9 +325,6 @@
   </si>
   <si>
     <t xml:space="preserve">genaue Dauer in Minuten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
   </si>
   <si>
     <t xml:space="preserve">meda_notiz</t>
@@ -1805,7 +1805,7 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
@@ -1813,10 +1813,10 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1827,10 +1827,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -1841,10 +1841,10 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -1855,10 +1855,10 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1869,13 +1869,13 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24">
@@ -1883,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1897,10 +1897,10 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1911,10 +1911,10 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1925,10 +1925,10 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1939,10 +1939,10 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -1953,10 +1953,10 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1967,10 +1967,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
         <v>28</v>
@@ -1981,10 +1981,10 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1995,13 +1995,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
@@ -2009,7 +2009,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -2079,10 +2079,10 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -2093,10 +2093,10 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -2107,10 +2107,10 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -2121,10 +2121,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -2135,10 +2135,10 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -2149,13 +2149,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44">
@@ -2163,10 +2163,10 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -2177,10 +2177,10 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -2191,10 +2191,10 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
@@ -2205,10 +2205,10 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -2219,10 +2219,10 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
         <v>28</v>
@@ -2233,10 +2233,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
@@ -2247,10 +2247,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -2261,10 +2261,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -2275,10 +2275,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -2289,10 +2289,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -2303,10 +2303,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -2317,10 +2317,10 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -2331,10 +2331,10 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -2345,10 +2345,10 @@
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -2359,13 +2359,13 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
@@ -2460,7 +2460,7 @@
         <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -2474,7 +2474,7 @@
         <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -2519,7 +2519,7 @@
         <v>115</v>
       </c>
       <c r="D69" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70">
@@ -3569,7 +3569,7 @@
         <v>257</v>
       </c>
       <c r="D144" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="145">
@@ -4003,7 +4003,7 @@
         <v>257</v>
       </c>
       <c r="D175" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="176">
@@ -4479,7 +4479,7 @@
         <v>329</v>
       </c>
       <c r="D209" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="210">
@@ -4493,7 +4493,7 @@
         <v>331</v>
       </c>
       <c r="D210" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="211">
@@ -4507,7 +4507,7 @@
         <v>333</v>
       </c>
       <c r="D211" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="212">
@@ -4521,7 +4521,7 @@
         <v>335</v>
       </c>
       <c r="D212" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="213">
@@ -4535,7 +4535,7 @@
         <v>337</v>
       </c>
       <c r="D213" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="214">
@@ -4549,7 +4549,7 @@
         <v>339</v>
       </c>
       <c r="D214" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="215">
@@ -4563,7 +4563,7 @@
         <v>341</v>
       </c>
       <c r="D215" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="216">
@@ -4577,7 +4577,7 @@
         <v>343</v>
       </c>
       <c r="D216" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="217">
@@ -4591,7 +4591,7 @@
         <v>345</v>
       </c>
       <c r="D217" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="218">
@@ -4605,7 +4605,7 @@
         <v>347</v>
       </c>
       <c r="D218" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="219">
@@ -4619,7 +4619,7 @@
         <v>349</v>
       </c>
       <c r="D219" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="220">
@@ -4633,7 +4633,7 @@
         <v>351</v>
       </c>
       <c r="D220" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="221">
@@ -4647,7 +4647,7 @@
         <v>353</v>
       </c>
       <c r="D221" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="222">
@@ -4745,7 +4745,7 @@
         <v>359</v>
       </c>
       <c r="D228" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="229">
@@ -4759,7 +4759,7 @@
         <v>361</v>
       </c>
       <c r="D229" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="230">
@@ -4773,7 +4773,7 @@
         <v>363</v>
       </c>
       <c r="D230" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="231">
@@ -4787,7 +4787,7 @@
         <v>365</v>
       </c>
       <c r="D231" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="232">
@@ -4801,7 +4801,7 @@
         <v>367</v>
       </c>
       <c r="D232" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="233">
@@ -4815,7 +4815,7 @@
         <v>369</v>
       </c>
       <c r="D233" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="234">
@@ -4829,7 +4829,7 @@
         <v>371</v>
       </c>
       <c r="D234" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="235">
@@ -4843,7 +4843,7 @@
         <v>373</v>
       </c>
       <c r="D235" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="236">
@@ -4857,7 +4857,7 @@
         <v>375</v>
       </c>
       <c r="D236" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="237">
@@ -4871,7 +4871,7 @@
         <v>377</v>
       </c>
       <c r="D237" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="238">
@@ -4885,7 +4885,7 @@
         <v>379</v>
       </c>
       <c r="D238" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="239">
@@ -4899,7 +4899,7 @@
         <v>381</v>
       </c>
       <c r="D239" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="240">
@@ -4913,7 +4913,7 @@
         <v>383</v>
       </c>
       <c r="D240" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="241">
@@ -4927,7 +4927,7 @@
         <v>385</v>
       </c>
       <c r="D241" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="242">
@@ -4941,7 +4941,7 @@
         <v>387</v>
       </c>
       <c r="D242" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="243">
@@ -4955,7 +4955,7 @@
         <v>389</v>
       </c>
       <c r="D243" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="244">
@@ -4969,7 +4969,7 @@
         <v>391</v>
       </c>
       <c r="D244" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="245">
@@ -4983,7 +4983,7 @@
         <v>393</v>
       </c>
       <c r="D245" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="246">
@@ -4997,7 +4997,7 @@
         <v>395</v>
       </c>
       <c r="D246" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="247">
@@ -5011,7 +5011,7 @@
         <v>397</v>
       </c>
       <c r="D247" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="248">
@@ -5025,7 +5025,7 @@
         <v>399</v>
       </c>
       <c r="D248" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="249">
@@ -5039,7 +5039,7 @@
         <v>401</v>
       </c>
       <c r="D249" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="250">

</xml_diff>